<commit_message>
creating a way to find to match   the others proponentes automatically
</commit_message>
<xml_diff>
--- a/Data_Dictionary/xlsx/Columns/Emendas_resumo_columns.xlsx
+++ b/Data_Dictionary/xlsx/Columns/Emendas_resumo_columns.xlsx
@@ -22,46 +22,46 @@
     <t>descricao</t>
   </si>
   <si>
+    <t>processo</t>
+  </si>
+  <si>
+    <t>emenda</t>
+  </si>
+  <si>
+    <t>valor</t>
+  </si>
+  <si>
+    <t>pontos_livre_(18_meses</t>
+  </si>
+  <si>
+    <t>pontos_gesac</t>
+  </si>
+  <si>
+    <t>pontos_indicados</t>
+  </si>
+  <si>
+    <t>pontos_analisados</t>
+  </si>
+  <si>
+    <t>pontos_aprovados</t>
+  </si>
+  <si>
+    <t>encaminhamento</t>
+  </si>
+  <si>
+    <t>data_aspar_informada</t>
+  </si>
+  <si>
+    <t>data_cadastrado</t>
+  </si>
+  <si>
+    <t>responsavel</t>
+  </si>
+  <si>
+    <t>pendencia_28/12</t>
+  </si>
+  <si>
     <t>proponente</t>
-  </si>
-  <si>
-    <t>processo</t>
-  </si>
-  <si>
-    <t>emenda</t>
-  </si>
-  <si>
-    <t>valor</t>
-  </si>
-  <si>
-    <t>pontos_livre_(18_meses</t>
-  </si>
-  <si>
-    <t>pontos_gesac</t>
-  </si>
-  <si>
-    <t>pontos_indicados</t>
-  </si>
-  <si>
-    <t>pontos_analisados</t>
-  </si>
-  <si>
-    <t>pontos_aprovados</t>
-  </si>
-  <si>
-    <t>encaminhamento</t>
-  </si>
-  <si>
-    <t>data_aspar_informada</t>
-  </si>
-  <si>
-    <t>data_cadastrado</t>
-  </si>
-  <si>
-    <t>responsavel</t>
-  </si>
-  <si>
-    <t>pendencia_28/12</t>
   </si>
   <si>
     <t>prop_pk1</t>

</xml_diff>